<commit_message>
a bit more update
</commit_message>
<xml_diff>
--- a/Work Breakdown Structure.xlsx
+++ b/Work Breakdown Structure.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3C86B7-BBB7-47A2-8E3D-04C4D24C520A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9630617-0B21-4B09-AF78-CE2F3F1B57B5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t>Task/Management</t>
   </si>
@@ -94,18 +94,6 @@
     <t>5.1 Close Project</t>
   </si>
   <si>
-    <t>5.3 Document report on departments' progress</t>
-  </si>
-  <si>
-    <t>5.4 Document report on obtained supplies/services</t>
-  </si>
-  <si>
-    <t>5.5 Document report on messeges/mails</t>
-  </si>
-  <si>
-    <t>5.6 Document report on losses</t>
-  </si>
-  <si>
     <t>2.3 Plan Communications Management</t>
   </si>
   <si>
@@ -146,6 +134,12 @@
   </si>
   <si>
     <t>4.4 Monitor and Control Risks</t>
+  </si>
+  <si>
+    <t>5.4 Document Procurement Report</t>
+  </si>
+  <si>
+    <t>5.6 Document Report on Losses</t>
   </si>
 </sst>
 </file>
@@ -477,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,7 +518,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -532,7 +526,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>5</v>
@@ -540,7 +534,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
@@ -548,7 +542,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
@@ -569,7 +563,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
@@ -577,7 +571,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -591,7 +585,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>5</v>
@@ -599,7 +593,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>5</v>
@@ -607,7 +601,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>5</v>
@@ -615,7 +609,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>5</v>
@@ -655,7 +649,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
@@ -709,7 +703,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
@@ -718,7 +712,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>5</v>
@@ -726,7 +720,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>5</v>
@@ -755,33 +749,17 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E41" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>